<commit_message>
Final update before submitting to PCB shop
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmbou\Source\eagle\nixie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7D495680-5353-4E78-B30B-7093C27BB59E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6936BC94-6E35-4A4A-9D99-13E55DDAD90A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7680" xr2:uid="{BFEC3CB6-2C13-4625-AB7A-A9B26EBADD8D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="133">
   <si>
     <t>Name</t>
   </si>
@@ -421,6 +421,9 @@
   </si>
   <si>
     <t>C1F 500</t>
+  </si>
+  <si>
+    <t>Phoenix Sep</t>
   </si>
 </sst>
 </file>
@@ -787,7 +790,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,6 +1264,9 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>132</v>
+      </c>
       <c r="B28" t="s">
         <v>111</v>
       </c>

</xml_diff>